<commit_message>
Fixed issue with DTaP
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/Diphtheria.xlsx
+++ b/src/main/webapp/schedules/Diphtheria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7533C466-4CC1-471E-8C99-85499DE2A1B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFA224D-DEA2-40B5-9AA0-C633DF88604E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32352" yWindow="-4008" windowWidth="17280" windowHeight="9240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -918,9 +921,6 @@
     <t>TCH</t>
   </si>
   <si>
-    <t>28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115</t>
-  </si>
-  <si>
     <t>09, 113, 115</t>
   </si>
   <si>
@@ -931,6 +931,9 @@
   </si>
   <si>
     <t>20, 110, 50, 120, 130, 22, 01, 120, 132, 115</t>
+  </si>
+  <si>
+    <t>28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115, 107, 106, 198</t>
   </si>
 </sst>
 </file>
@@ -3505,7 +3508,7 @@
   <dimension ref="B1:J357"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3560,7 +3563,7 @@
       <c r="H3" s="52"/>
       <c r="I3" s="35"/>
       <c r="J3" s="55" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -3568,7 +3571,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D4" s="59"/>
       <c r="F4" s="36" t="s">
@@ -3600,7 +3603,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D6" s="37"/>
       <c r="F6" s="36" t="s">
@@ -3618,7 +3621,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D7" s="39"/>
       <c r="F7" s="36" t="s">
@@ -3636,7 +3639,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="40" t="s">
@@ -6826,15 +6829,17 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="36">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="B348:D348"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B319:E319"/>
+    <mergeCell ref="B328:D328"/>
+    <mergeCell ref="B296:E296"/>
+    <mergeCell ref="B276:E276"/>
+    <mergeCell ref="B228:D228"/>
+    <mergeCell ref="B199:E199"/>
+    <mergeCell ref="B208:D208"/>
     <mergeCell ref="B150:D150"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="B72:D72"/>
@@ -6851,17 +6856,15 @@
     <mergeCell ref="B238:E238"/>
     <mergeCell ref="B265:D265"/>
     <mergeCell ref="B247:D247"/>
-    <mergeCell ref="B348:D348"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B319:E319"/>
-    <mergeCell ref="B328:D328"/>
-    <mergeCell ref="B296:E296"/>
-    <mergeCell ref="B276:E276"/>
-    <mergeCell ref="B228:D228"/>
-    <mergeCell ref="B199:E199"/>
-    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6905,7 +6908,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115, 107, 106, 198"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
LSVF-5 Fixed valid grace period to include 12 months
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/Diphtheria.xlsx
+++ b/src/main/webapp/schedules/Diphtheria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3966257D-72B7-4F5F-A12F-A69FCA5764D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0382B8EB-E53D-43F8-B988-92E510811B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10635" yWindow="-15945" windowWidth="17805" windowHeight="10425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="299">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -931,6 +931,9 @@
   </si>
   <si>
     <t>28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115, 107, 106, 198</t>
+  </si>
+  <si>
+    <t>3 months 4 days</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1330,6 +1333,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3502,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4473,8 +4479,8 @@
       <c r="D124" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E124" s="36" t="s">
-        <v>19</v>
+      <c r="E124" s="59" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
@@ -6824,15 +6830,17 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="36">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="B348:D348"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B319:E319"/>
+    <mergeCell ref="B328:D328"/>
+    <mergeCell ref="B296:E296"/>
+    <mergeCell ref="B276:E276"/>
+    <mergeCell ref="B228:D228"/>
+    <mergeCell ref="B199:E199"/>
+    <mergeCell ref="B208:D208"/>
     <mergeCell ref="B150:D150"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="B72:D72"/>
@@ -6849,17 +6857,15 @@
     <mergeCell ref="B238:E238"/>
     <mergeCell ref="B265:D265"/>
     <mergeCell ref="B247:D247"/>
-    <mergeCell ref="B348:D348"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B319:E319"/>
-    <mergeCell ref="B328:D328"/>
-    <mergeCell ref="B296:E296"/>
-    <mergeCell ref="B276:E276"/>
-    <mergeCell ref="B228:D228"/>
-    <mergeCell ref="B199:E199"/>
-    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7223,7 +7229,7 @@
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C124&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E124&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="15 months" interval="6 months" grace="2 months"/&gt;</v>
+        <v xml:space="preserve">    &lt;valid age="15 months" interval="6 months" grace="3 months 4 days"/&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
LSFV-7 Removed Tdap from childhood list
</commit_message>
<xml_diff>
--- a/src/main/webapp/schedules/Diphtheria.xlsx
+++ b/src/main/webapp/schedules/Diphtheria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenyon\Documents\GitHub\LoneStarVaccineForecaster\src\main\webapp\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\tch\forecaster\src\main\webapp\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B8769E-BC27-4F52-A26A-1D4DCA095CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8599D2E4-BB15-4D07-9D9D-D976593CB071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp" sheetId="6" r:id="rId1"/>
@@ -930,9 +930,6 @@
     <t>20, 110, 50, 120, 130, 22, 01, 120, 132, 115</t>
   </si>
   <si>
-    <t>28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115, 107, 106, 198</t>
-  </si>
-  <si>
     <t>3 months 4 days</t>
   </si>
   <si>
@@ -940,6 +937,9 @@
   </si>
   <si>
     <t>2 months 4 days</t>
+  </si>
+  <si>
+    <t>28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 107, 106, 198</t>
   </si>
 </sst>
 </file>
@@ -1328,6 +1328,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1341,9 +1344,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3517,8 +3517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3550,13 +3550,13 @@
       <c r="D2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="31" t="s">
@@ -3577,13 +3577,13 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="57" t="s">
-        <v>297</v>
-      </c>
-      <c r="D4" s="58"/>
+      <c r="C4" s="58" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="59"/>
       <c r="F4" s="34" t="s">
         <v>286</v>
       </c>
@@ -3595,9 +3595,9 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="56"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
       <c r="F5" s="34" t="s">
         <v>6</v>
       </c>
@@ -3645,13 +3645,13 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="D8" s="58"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="38" t="s">
         <v>46</v>
       </c>
@@ -3666,9 +3666,9 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="56"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
       <c r="F9" s="34" t="s">
         <v>12</v>
       </c>
@@ -3755,11 +3755,11 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
       <c r="F15" s="34" t="s">
         <v>280</v>
       </c>
@@ -3879,12 +3879,12 @@
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B63" s="55" t="s">
+      <c r="B63" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="44"/>
@@ -3969,11 +3969,11 @@
       <c r="E71" s="36"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B72" s="55" t="s">
+      <c r="B72" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="56"/>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" s="31" t="s">
@@ -4066,12 +4066,12 @@
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B83" s="55" t="s">
+      <c r="B83" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C83" s="55"/>
-      <c r="D83" s="55"/>
-      <c r="E83" s="55"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="44"/>
@@ -4158,11 +4158,11 @@
       <c r="E91" s="36"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B92" s="55" t="s">
+      <c r="B92" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C92" s="55"/>
-      <c r="D92" s="55"/>
+      <c r="C92" s="56"/>
+      <c r="D92" s="56"/>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B93" s="31" t="s">
@@ -4255,12 +4255,12 @@
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B102" s="55" t="s">
+      <c r="B102" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C102" s="55"/>
-      <c r="D102" s="55"/>
-      <c r="E102" s="55"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="56"/>
+      <c r="E102" s="56"/>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="44"/>
@@ -4347,11 +4347,11 @@
       <c r="E110" s="36"/>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B111" s="55" t="s">
+      <c r="B111" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C111" s="55"/>
-      <c r="D111" s="55"/>
+      <c r="C111" s="56"/>
+      <c r="D111" s="56"/>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="31" t="s">
@@ -4459,12 +4459,12 @@
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B122" s="55" t="s">
+      <c r="B122" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C122" s="55"/>
-      <c r="D122" s="55"/>
-      <c r="E122" s="55"/>
+      <c r="C122" s="56"/>
+      <c r="D122" s="56"/>
+      <c r="E122" s="56"/>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="44"/>
@@ -4478,7 +4478,7 @@
         <v>27</v>
       </c>
       <c r="F123" s="53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
@@ -4492,10 +4492,10 @@
         <v>52</v>
       </c>
       <c r="E124" s="54" t="s">
-        <v>298</v>
-      </c>
-      <c r="F124" s="60" t="s">
-        <v>300</v>
+        <v>297</v>
+      </c>
+      <c r="F124" s="55" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
@@ -4559,11 +4559,11 @@
       <c r="E130" s="36"/>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B131" s="55" t="s">
+      <c r="B131" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C131" s="55"/>
-      <c r="D131" s="55"/>
+      <c r="C131" s="56"/>
+      <c r="D131" s="56"/>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="31" t="s">
@@ -4656,12 +4656,12 @@
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B141" s="55" t="s">
+      <c r="B141" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C141" s="55"/>
-      <c r="D141" s="55"/>
-      <c r="E141" s="55"/>
+      <c r="C141" s="56"/>
+      <c r="D141" s="56"/>
+      <c r="E141" s="56"/>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="44"/>
@@ -4746,11 +4746,11 @@
       <c r="E149" s="36"/>
     </row>
     <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B150" s="55" t="s">
+      <c r="B150" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C150" s="55"/>
-      <c r="D150" s="55"/>
+      <c r="C150" s="56"/>
+      <c r="D150" s="56"/>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B151" s="31" t="s">
@@ -4843,12 +4843,12 @@
       </c>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B160" s="55" t="s">
+      <c r="B160" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C160" s="55"/>
-      <c r="D160" s="55"/>
-      <c r="E160" s="55"/>
+      <c r="C160" s="56"/>
+      <c r="D160" s="56"/>
+      <c r="E160" s="56"/>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B161" s="44"/>
@@ -4933,11 +4933,11 @@
       <c r="E168" s="36"/>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B169" s="55" t="s">
+      <c r="B169" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C169" s="55"/>
-      <c r="D169" s="55"/>
+      <c r="C169" s="56"/>
+      <c r="D169" s="56"/>
     </row>
     <row r="170" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B170" s="31" t="s">
@@ -5028,12 +5028,12 @@
       </c>
     </row>
     <row r="179" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B179" s="55" t="s">
+      <c r="B179" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C179" s="55"/>
-      <c r="D179" s="55"/>
-      <c r="E179" s="55"/>
+      <c r="C179" s="56"/>
+      <c r="D179" s="56"/>
+      <c r="E179" s="56"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B180" s="44"/>
@@ -5118,11 +5118,11 @@
       <c r="E187" s="36"/>
     </row>
     <row r="188" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B188" s="55" t="s">
+      <c r="B188" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C188" s="55"/>
-      <c r="D188" s="55"/>
+      <c r="C188" s="56"/>
+      <c r="D188" s="56"/>
     </row>
     <row r="189" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B189" s="31" t="s">
@@ -5228,12 +5228,12 @@
       </c>
     </row>
     <row r="199" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B199" s="55" t="s">
+      <c r="B199" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C199" s="55"/>
-      <c r="D199" s="55"/>
-      <c r="E199" s="55"/>
+      <c r="C199" s="56"/>
+      <c r="D199" s="56"/>
+      <c r="E199" s="56"/>
     </row>
     <row r="200" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B200" s="44"/>
@@ -5320,11 +5320,11 @@
       <c r="E207" s="36"/>
     </row>
     <row r="208" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B208" s="55" t="s">
+      <c r="B208" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C208" s="55"/>
-      <c r="D208" s="55"/>
+      <c r="C208" s="56"/>
+      <c r="D208" s="56"/>
     </row>
     <row r="209" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B209" s="31" t="s">
@@ -5417,12 +5417,12 @@
       </c>
     </row>
     <row r="218" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B218" s="55" t="s">
+      <c r="B218" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C218" s="55"/>
-      <c r="D218" s="55"/>
-      <c r="E218" s="55"/>
+      <c r="C218" s="56"/>
+      <c r="D218" s="56"/>
+      <c r="E218" s="56"/>
     </row>
     <row r="219" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B219" s="44"/>
@@ -5519,11 +5519,11 @@
       <c r="E227" s="36"/>
     </row>
     <row r="228" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B228" s="55" t="s">
+      <c r="B228" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C228" s="55"/>
-      <c r="D228" s="55"/>
+      <c r="C228" s="56"/>
+      <c r="D228" s="56"/>
     </row>
     <row r="229" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B229" s="31" t="s">
@@ -5616,12 +5616,12 @@
       </c>
     </row>
     <row r="238" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B238" s="55" t="s">
+      <c r="B238" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C238" s="55"/>
-      <c r="D238" s="55"/>
-      <c r="E238" s="55"/>
+      <c r="C238" s="56"/>
+      <c r="D238" s="56"/>
+      <c r="E238" s="56"/>
     </row>
     <row r="239" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B239" s="44"/>
@@ -5706,11 +5706,11 @@
       <c r="E246" s="36"/>
     </row>
     <row r="247" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B247" s="55" t="s">
+      <c r="B247" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C247" s="55"/>
-      <c r="D247" s="55"/>
+      <c r="C247" s="56"/>
+      <c r="D247" s="56"/>
     </row>
     <row r="248" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B248" s="31" t="s">
@@ -5790,12 +5790,12 @@
       </c>
     </row>
     <row r="256" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B256" s="55" t="s">
+      <c r="B256" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C256" s="55"/>
-      <c r="D256" s="55"/>
-      <c r="E256" s="55"/>
+      <c r="C256" s="56"/>
+      <c r="D256" s="56"/>
+      <c r="E256" s="56"/>
     </row>
     <row r="257" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B257" s="44"/>
@@ -5878,11 +5878,11 @@
       <c r="E264" s="36"/>
     </row>
     <row r="265" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B265" s="55" t="s">
+      <c r="B265" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C265" s="55"/>
-      <c r="D265" s="55"/>
+      <c r="C265" s="56"/>
+      <c r="D265" s="56"/>
     </row>
     <row r="266" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B266" s="31" t="s">
@@ -5990,12 +5990,12 @@
       </c>
     </row>
     <row r="276" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B276" s="55" t="s">
+      <c r="B276" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C276" s="55"/>
-      <c r="D276" s="55"/>
-      <c r="E276" s="55"/>
+      <c r="C276" s="56"/>
+      <c r="D276" s="56"/>
+      <c r="E276" s="56"/>
     </row>
     <row r="277" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B277" s="44"/>
@@ -6080,11 +6080,11 @@
       <c r="E284" s="36"/>
     </row>
     <row r="285" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B285" s="55" t="s">
+      <c r="B285" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C285" s="55"/>
-      <c r="D285" s="55"/>
+      <c r="C285" s="56"/>
+      <c r="D285" s="56"/>
     </row>
     <row r="286" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B286" s="31" t="s">
@@ -6192,12 +6192,12 @@
       </c>
     </row>
     <row r="296" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B296" s="55" t="s">
+      <c r="B296" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C296" s="55"/>
-      <c r="D296" s="55"/>
-      <c r="E296" s="55"/>
+      <c r="C296" s="56"/>
+      <c r="D296" s="56"/>
+      <c r="E296" s="56"/>
     </row>
     <row r="297" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B297" s="44"/>
@@ -6284,11 +6284,11 @@
       <c r="E304" s="36"/>
     </row>
     <row r="305" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B305" s="55" t="s">
+      <c r="B305" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C305" s="55"/>
-      <c r="D305" s="55"/>
+      <c r="C305" s="56"/>
+      <c r="D305" s="56"/>
     </row>
     <row r="306" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B306" s="31" t="s">
@@ -6437,12 +6437,12 @@
       </c>
     </row>
     <row r="319" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B319" s="55" t="s">
+      <c r="B319" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C319" s="55"/>
-      <c r="D319" s="55"/>
-      <c r="E319" s="55"/>
+      <c r="C319" s="56"/>
+      <c r="D319" s="56"/>
+      <c r="E319" s="56"/>
     </row>
     <row r="320" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B320" s="44"/>
@@ -6525,11 +6525,11 @@
       <c r="E327" s="36"/>
     </row>
     <row r="328" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B328" s="55" t="s">
+      <c r="B328" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C328" s="55"/>
-      <c r="D328" s="55"/>
+      <c r="C328" s="56"/>
+      <c r="D328" s="56"/>
     </row>
     <row r="329" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B329" s="31" t="s">
@@ -6635,12 +6635,12 @@
       </c>
     </row>
     <row r="339" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B339" s="55" t="s">
+      <c r="B339" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C339" s="55"/>
-      <c r="D339" s="55"/>
-      <c r="E339" s="55"/>
+      <c r="C339" s="56"/>
+      <c r="D339" s="56"/>
+      <c r="E339" s="56"/>
     </row>
     <row r="340" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B340" s="44"/>
@@ -6723,11 +6723,11 @@
       <c r="E347" s="36"/>
     </row>
     <row r="348" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B348" s="55" t="s">
+      <c r="B348" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="C348" s="55"/>
-      <c r="D348" s="55"/>
+      <c r="C348" s="56"/>
+      <c r="D348" s="56"/>
     </row>
     <row r="349" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B349" s="31" t="s">
@@ -6845,15 +6845,17 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="36">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B141:E141"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="B348:D348"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="B179:E179"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B319:E319"/>
+    <mergeCell ref="B328:D328"/>
+    <mergeCell ref="B296:E296"/>
+    <mergeCell ref="B276:E276"/>
+    <mergeCell ref="B228:D228"/>
+    <mergeCell ref="B199:E199"/>
+    <mergeCell ref="B208:D208"/>
     <mergeCell ref="B150:D150"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="B72:D72"/>
@@ -6870,17 +6872,15 @@
     <mergeCell ref="B238:E238"/>
     <mergeCell ref="B265:D265"/>
     <mergeCell ref="B247:D247"/>
-    <mergeCell ref="B348:D348"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="B179:E179"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B319:E319"/>
-    <mergeCell ref="B328:D328"/>
-    <mergeCell ref="B296:E296"/>
-    <mergeCell ref="B276:E276"/>
-    <mergeCell ref="B228:D228"/>
-    <mergeCell ref="B199:E199"/>
-    <mergeCell ref="B208:D208"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B141:E141"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6908,8 +6908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6926,7 +6926,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 115, 107, 106, 198"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="28, 20, 110, 50, 120, 130, 22, 01, 102, 120, 132, 107, 106, 198"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -8281,10 +8281,10 @@
       <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="3" t="s">
         <v>76</v>
       </c>
@@ -9208,10 +9208,10 @@
       <c r="B28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="3" t="s">
         <v>76</v>
       </c>
@@ -9227,10 +9227,10 @@
       <c r="J28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K28" s="59" t="s">
+      <c r="K28" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="L28" s="59"/>
+      <c r="L28" s="60"/>
       <c r="N28" s="6" t="s">
         <v>77</v>
       </c>

</xml_diff>